<commit_message>
Made some changes in tables
</commit_message>
<xml_diff>
--- a/DB/CI_TABLES.xlsx
+++ b/DB/CI_TABLES.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="119">
   <si>
     <t>Field</t>
   </si>
@@ -52,9 +52,6 @@
     <t>none</t>
   </si>
   <si>
-    <t>auto increment</t>
-  </si>
-  <si>
     <t>unassigned</t>
   </si>
   <si>
@@ -235,9 +232,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>Table : Mission_Skill</t>
-  </si>
-  <si>
     <t xml:space="preserve"> skill_id</t>
   </si>
   <si>
@@ -299,6 +293,84 @@
   </si>
   <si>
     <t>Table : User</t>
+  </si>
+  <si>
+    <t>Table : Country</t>
+  </si>
+  <si>
+    <t>Table : City</t>
+  </si>
+  <si>
+    <t>Table : Skill</t>
+  </si>
+  <si>
+    <t>Table : Story</t>
+  </si>
+  <si>
+    <t>story_id</t>
+  </si>
+  <si>
+    <t>foreignkey(user)</t>
+  </si>
+  <si>
+    <t>foreignkey(mission)</t>
+  </si>
+  <si>
+    <t>story_title</t>
+  </si>
+  <si>
+    <t>photos</t>
+  </si>
+  <si>
+    <t>videos</t>
+  </si>
+  <si>
+    <t>Table : Story_Application</t>
+  </si>
+  <si>
+    <t>foreignkey(story)</t>
+  </si>
+  <si>
+    <t>approved_status</t>
+  </si>
+  <si>
+    <t>Table : Volunteer_Timesheet</t>
+  </si>
+  <si>
+    <t>vol_date</t>
+  </si>
+  <si>
+    <t>vol_hours</t>
+  </si>
+  <si>
+    <t>vol_minutes</t>
+  </si>
+  <si>
+    <t>message</t>
+  </si>
+  <si>
+    <t>Table : ContactUs</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>messsage</t>
+  </si>
+  <si>
+    <t>UNSIGNED</t>
+  </si>
+  <si>
+    <t>auto_increment</t>
+  </si>
+  <si>
+    <t>Table : Banner_Management</t>
+  </si>
+  <si>
+    <t>banner_id</t>
+  </si>
+  <si>
+    <t>primary_key</t>
   </si>
 </sst>
 </file>
@@ -467,11 +539,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -482,6 +549,11 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -699,25 +771,25 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:H153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K78" sqref="K78"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="8"/>
+      <c r="A1" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="11"/>
     </row>
     <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -749,8 +821,8 @@
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="10" t="s">
-        <v>36</v>
+      <c r="B3" s="7" t="s">
+        <v>35</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="4" t="s">
@@ -759,22 +831,22 @@
       <c r="E3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>16</v>
       </c>
       <c r="C4" s="4">
         <v>50</v>
@@ -782,7 +854,7 @@
       <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F4" s="5"/>
@@ -791,10 +863,10 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="4">
         <v>50</v>
@@ -802,7 +874,7 @@
       <c r="D5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="5"/>
@@ -811,10 +883,10 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
@@ -831,17 +903,17 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>65</v>
+        <v>19</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -849,10 +921,10 @@
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C8" s="4">
         <v>50</v>
@@ -865,16 +937,16 @@
       </c>
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
-      <c r="H8" s="11" t="s">
-        <v>39</v>
+      <c r="H8" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
         <v>255</v>
@@ -882,7 +954,7 @@
       <c r="D9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="5"/>
@@ -891,17 +963,17 @@
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="4" t="s">
         <v>24</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>25</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
@@ -909,17 +981,17 @@
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
@@ -927,33 +999,33 @@
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
+      <c r="A16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="10"/>
+      <c r="D16" s="10"/>
+      <c r="E16" s="10"/>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
@@ -982,39 +1054,41 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="B18" s="10" t="s">
+      <c r="A18" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="11"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="4"/>
+      <c r="F18" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="G18" s="4"/>
-      <c r="H18" s="10" t="s">
-        <v>59</v>
+      <c r="H18" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" s="11">
+        <v>55</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="8">
         <v>50</v>
       </c>
-      <c r="D19" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="4"/>
@@ -1023,50 +1097,50 @@
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C20" s="4">
         <v>255</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="9" t="s">
-        <v>32</v>
+      <c r="A21" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="4">
         <v>50</v>
       </c>
-      <c r="D21" s="10" t="s">
-        <v>21</v>
+      <c r="D21" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4" t="s">
@@ -1080,16 +1154,16 @@
       <c r="H22" s="5"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="8"/>
+      <c r="A25" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="11"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
@@ -1118,39 +1192,41 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="10" t="s">
+      <c r="A27" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="11"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="4"/>
+      <c r="F27" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="G27" s="4"/>
-      <c r="H27" s="10" t="s">
-        <v>14</v>
+      <c r="H27" s="7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9" t="s">
+      <c r="A28" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="8">
         <v>50</v>
       </c>
-      <c r="B28" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="11">
-        <v>50</v>
-      </c>
-      <c r="D28" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="D28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F28" s="4"/>
@@ -1158,50 +1234,50 @@
       <c r="H28" s="4"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="9" t="s">
-        <v>49</v>
+      <c r="A29" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C29" s="4">
         <v>100</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="9" t="s">
-        <v>48</v>
+      <c r="A30" s="6" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C30" s="4">
         <v>255</v>
       </c>
-      <c r="D30" s="10" t="s">
-        <v>21</v>
+      <c r="D30" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31" s="10" t="s">
+      <c r="A31" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C31" s="4"/>
@@ -1212,83 +1288,87 @@
         <v>11</v>
       </c>
       <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="11" t="s">
+      <c r="G31" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="B33" s="10" t="s">
-        <v>16</v>
+      <c r="A33" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="C33" s="4">
         <v>15</v>
       </c>
-      <c r="D33" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>17</v>
+      <c r="D33" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
       <c r="H33" s="5"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="A34" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34" s="4">
+        <v>255</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="C34" s="4">
-        <v>15</v>
-      </c>
-      <c r="D34" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>17</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
       <c r="H34" s="5"/>
     </row>
     <row r="35" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="9" t="s">
+      <c r="A35" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="C35" s="4"/>
-      <c r="D35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E35" s="10" t="s">
+      <c r="D35" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F35" s="5"/>
@@ -1296,17 +1376,17 @@
       <c r="H35" s="5"/>
     </row>
     <row r="36" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="B36" s="10" t="s">
-        <v>44</v>
+      <c r="A36" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C36" s="4"/>
-      <c r="D36" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="10" t="s">
+      <c r="D36" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F36" s="5"/>
@@ -1314,19 +1394,19 @@
       <c r="H36" s="5"/>
     </row>
     <row r="37" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
+      <c r="A37" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>51</v>
-      </c>
-      <c r="B37" s="10" t="s">
-        <v>52</v>
       </c>
       <c r="C37" s="4">
         <v>5</v>
       </c>
-      <c r="D37" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="10" t="s">
+      <c r="D37" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F37" s="5"/>
@@ -1334,131 +1414,135 @@
       <c r="H37" s="5"/>
     </row>
     <row r="38" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="10" t="s">
+      <c r="A38" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C38" s="4"/>
-      <c r="D38" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>17</v>
+      <c r="D38" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E38" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
       <c r="H38" s="5"/>
     </row>
     <row r="39" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="B39" s="10" t="s">
-        <v>44</v>
+      <c r="A39" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="C39" s="4"/>
-      <c r="D39" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>17</v>
+      <c r="D39" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
       <c r="H39" s="5"/>
     </row>
     <row r="40" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+      <c r="A40" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="4"/>
+      <c r="D40" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F40" s="5"/>
+      <c r="G40" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="B40" s="10" t="s">
+    </row>
+    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="9" t="s">
+      <c r="C41" s="4"/>
+      <c r="D41" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F41" s="5"/>
+      <c r="G41" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H41" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B41" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="11" t="s">
+    </row>
+    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="6" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="9" t="s">
+      <c r="B42" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="B42" s="10" t="s">
-        <v>65</v>
-      </c>
       <c r="C42" s="4"/>
-      <c r="D42" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>17</v>
+      <c r="D42" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E42" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
     </row>
     <row r="43" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>69</v>
+      <c r="A43" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C43" s="4"/>
-      <c r="D43" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E43" s="10" t="s">
-        <v>17</v>
+      <c r="D43" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
     </row>
     <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>52</v>
+      <c r="A44" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C44" s="4">
         <v>20</v>
       </c>
-      <c r="D44" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="10" t="s">
+      <c r="D44" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F44" s="5"/>
@@ -1466,34 +1550,34 @@
       <c r="H44" s="5"/>
     </row>
     <row r="45" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="9" t="s">
+      <c r="A45" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B45" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B45" s="10" t="s">
-        <v>69</v>
-      </c>
       <c r="C45" s="4"/>
-      <c r="D45" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E45" s="10" t="s">
-        <v>17</v>
+      <c r="D45" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E45" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
     </row>
     <row r="48" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="B48" s="7"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="7"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="8"/>
+      <c r="A48" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="B48" s="10"/>
+      <c r="C48" s="10"/>
+      <c r="D48" s="10"/>
+      <c r="E48" s="10"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="11"/>
     </row>
     <row r="49" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
@@ -1522,39 +1606,41 @@
       </c>
     </row>
     <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="9" t="s">
+      <c r="A50" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" s="8"/>
+      <c r="D50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F50" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G50" s="4"/>
+      <c r="H50" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" s="11"/>
-      <c r="D50" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C51" s="11">
+      <c r="B51" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D51" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E51" s="10" t="s">
+      <c r="C51" s="8">
+        <v>15</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F51" s="4"/>
@@ -1562,19 +1648,17 @@
       <c r="H51" s="4"/>
     </row>
     <row r="52" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="9" t="s">
+      <c r="A52" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B52" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C52" s="4">
-        <v>0</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="10" t="s">
+      <c r="C52" s="4"/>
+      <c r="D52" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F52" s="5"/>
@@ -1582,16 +1666,16 @@
       <c r="H52" s="5"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="12" t="s">
-        <v>73</v>
-      </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="7"/>
-      <c r="D55" s="7"/>
-      <c r="E55" s="7"/>
-      <c r="F55" s="7"/>
-      <c r="G55" s="7"/>
-      <c r="H55" s="8"/>
+      <c r="A55" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="10"/>
+      <c r="E55" s="10"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="11"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
@@ -1620,39 +1704,41 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="B57" s="10" t="s">
+      <c r="A57" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C57" s="11"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F57" s="4"/>
+      <c r="F57" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="G57" s="4"/>
-      <c r="H57" s="10" t="s">
-        <v>59</v>
+      <c r="H57" s="7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B58" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C58" s="11">
+      <c r="A58" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E58" s="10" t="s">
+      <c r="C58" s="8">
+        <v>15</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F58" s="4"/>
@@ -1660,16 +1746,16 @@
       <c r="H58" s="4"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="B61" s="7"/>
-      <c r="C61" s="7"/>
-      <c r="D61" s="7"/>
-      <c r="E61" s="7"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="8"/>
+      <c r="A61" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="10"/>
+      <c r="E61" s="10"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="10"/>
+      <c r="H61" s="11"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
@@ -1698,79 +1784,79 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" s="8"/>
+      <c r="D63" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E63" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H63" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="10" t="s">
+    </row>
+    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B64" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C63" s="11"/>
-      <c r="D63" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F63" s="4"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="9" t="s">
+      <c r="C64" s="8"/>
+      <c r="D64" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H64" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" s="11">
-        <v>15</v>
-      </c>
-      <c r="D64" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E64" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="10" t="s">
+    </row>
+    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="6" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="9" t="s">
-        <v>81</v>
-      </c>
-      <c r="B65" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C65" s="11"/>
-      <c r="D65" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E65" s="10" t="s">
-        <v>26</v>
+      <c r="B65" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C65" s="8"/>
+      <c r="D65" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
-      <c r="H65" s="10"/>
+      <c r="H65" s="7"/>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="B66" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C66" s="4">
-        <v>0</v>
-      </c>
-      <c r="D66" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E66" s="10" t="s">
+      <c r="A66" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B66" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E66" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F66" s="5"/>
@@ -1778,16 +1864,16 @@
       <c r="H66" s="5"/>
     </row>
     <row r="69" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="B69" s="7"/>
-      <c r="C69" s="7"/>
-      <c r="D69" s="7"/>
-      <c r="E69" s="7"/>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="8"/>
+      <c r="A69" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="10"/>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
+      <c r="G69" s="10"/>
+      <c r="H69" s="11"/>
     </row>
     <row r="70" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
@@ -1816,77 +1902,79 @@
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="9" t="s">
+      <c r="A71" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="8"/>
+      <c r="D71" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H71" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="B71" s="10" t="s">
+    </row>
+    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B72" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C71" s="11"/>
-      <c r="D71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E71" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="10" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9" t="s">
+      <c r="C72" s="8"/>
+      <c r="D72" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H72" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B72" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" s="11">
-        <v>15</v>
-      </c>
-      <c r="D72" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F72" s="4"/>
-      <c r="G72" s="4"/>
-      <c r="H72" s="10" t="s">
-        <v>79</v>
-      </c>
     </row>
     <row r="73" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="B73" s="10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C73" s="11"/>
-      <c r="D73" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>26</v>
+      <c r="A73" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B73" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73" s="8"/>
+      <c r="D73" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F73" s="4"/>
       <c r="G73" s="4"/>
-      <c r="H73" s="10"/>
+      <c r="H73" s="7"/>
     </row>
     <row r="74" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A74" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74" s="10" t="s">
+      <c r="A74" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B74" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C74" s="4"/>
-      <c r="D74" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E74" s="10" t="s">
+      <c r="D74" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E74" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F74" s="5"/>
@@ -1894,16 +1982,16 @@
       <c r="H74" s="5"/>
     </row>
     <row r="77" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="B77" s="7"/>
-      <c r="C77" s="7"/>
-      <c r="D77" s="7"/>
-      <c r="E77" s="7"/>
-      <c r="F77" s="7"/>
-      <c r="G77" s="7"/>
-      <c r="H77" s="8"/>
+      <c r="A77" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77" s="10"/>
+      <c r="C77" s="10"/>
+      <c r="D77" s="10"/>
+      <c r="E77" s="10"/>
+      <c r="F77" s="10"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="11"/>
     </row>
     <row r="78" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
@@ -1932,39 +2020,41 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A79" s="9" t="s">
-        <v>77</v>
-      </c>
-      <c r="B79" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C79" s="11"/>
+      <c r="A79" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C79" s="8"/>
       <c r="D79" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E79" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="4"/>
+      <c r="F79" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="G79" s="4"/>
-      <c r="H79" s="10" t="s">
+      <c r="H79" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B80" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C80" s="11">
+      <c r="B80" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C80" s="8">
         <v>16</v>
       </c>
-      <c r="D80" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" s="10" t="s">
+      <c r="D80" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E80" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F80" s="4"/>
@@ -1972,53 +2062,53 @@
       <c r="H80" s="4"/>
     </row>
     <row r="81" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B81" s="10" t="s">
-        <v>52</v>
+      <c r="A81" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C81" s="4">
         <v>16</v>
       </c>
-      <c r="D81" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" s="10" t="s">
-        <v>53</v>
+      <c r="D81" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>52</v>
       </c>
       <c r="F81" s="5"/>
       <c r="G81" s="5"/>
       <c r="H81" s="5"/>
     </row>
     <row r="82" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B82" s="10" t="s">
-        <v>52</v>
+      <c r="A82" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B82" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C82" s="4">
         <v>30</v>
       </c>
-      <c r="D82" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" s="10" t="s">
+      <c r="D82" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E82" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F82" s="5"/>
       <c r="G82" s="5"/>
-      <c r="H82" s="11" t="s">
-        <v>93</v>
+      <c r="H82" s="8" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B83" s="10" t="s">
-        <v>52</v>
+      <c r="A83" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C83" s="4"/>
       <c r="D83" s="4" t="s">
@@ -2029,76 +2119,76 @@
       </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
-      <c r="H83" s="11"/>
+      <c r="H83" s="8"/>
     </row>
     <row r="84" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B84" s="10" t="s">
+      <c r="A84" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B84" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C84" s="4"/>
-      <c r="D84" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" s="10" t="s">
+      <c r="D84" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E84" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
-      <c r="H84" s="11"/>
+      <c r="H84" s="8"/>
     </row>
     <row r="85" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="B85" s="10" t="s">
-        <v>65</v>
+      <c r="A85" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="C85" s="4">
         <v>15</v>
       </c>
-      <c r="D85" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E85" s="10" t="s">
-        <v>17</v>
+      <c r="D85" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F85" s="5"/>
       <c r="G85" s="5"/>
       <c r="H85" s="5"/>
     </row>
     <row r="86" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B86" s="10" t="s">
-        <v>69</v>
+      <c r="A86" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C86" s="4"/>
-      <c r="D86" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E86" s="10" t="s">
-        <v>17</v>
+      <c r="D86" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E86" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F86" s="5"/>
       <c r="G86" s="5"/>
       <c r="H86" s="5"/>
     </row>
     <row r="87" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="B87" s="10" t="s">
+      <c r="A87" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="7" t="s">
         <v>9</v>
       </c>
       <c r="C87" s="4"/>
-      <c r="D87" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E87" s="10" t="s">
+      <c r="D87" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E87" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F87" s="5"/>
@@ -2106,19 +2196,19 @@
       <c r="H87" s="5"/>
     </row>
     <row r="88" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="B88" s="10" t="s">
-        <v>52</v>
+      <c r="A88" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C88" s="4">
         <v>5</v>
       </c>
-      <c r="D88" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E88" s="10" t="s">
+      <c r="D88" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E88" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F88" s="5"/>
@@ -2126,115 +2216,119 @@
       <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="9" t="s">
+      <c r="A89" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C89" s="4"/>
+      <c r="D89" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="5"/>
+      <c r="G89" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H89" s="8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B90" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C89" s="4"/>
-      <c r="D89" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E89" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="5"/>
-      <c r="G89" s="5"/>
-      <c r="H89" s="11" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B90" s="10" t="s">
+      <c r="C90" s="4"/>
+      <c r="D90" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E90" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="5"/>
+      <c r="G90" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H90" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="C90" s="4"/>
-      <c r="D90" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E90" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="5"/>
-      <c r="G90" s="5"/>
-      <c r="H90" s="11" t="s">
-        <v>45</v>
-      </c>
     </row>
     <row r="91" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="B91" s="10" t="s">
-        <v>69</v>
+      <c r="A91" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C91" s="4"/>
-      <c r="D91" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E91" s="10" t="s">
-        <v>17</v>
+      <c r="D91" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E91" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F91" s="5"/>
       <c r="G91" s="5"/>
-      <c r="H91" s="11"/>
+      <c r="H91" s="8"/>
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B92" s="10" t="s">
-        <v>52</v>
+      <c r="A92" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="B92" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C92" s="4">
         <v>255</v>
       </c>
-      <c r="D92" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E92" s="10" t="s">
-        <v>17</v>
+      <c r="D92" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E92" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F92" s="5"/>
       <c r="G92" s="5"/>
-      <c r="H92" s="11"/>
+      <c r="H92" s="8"/>
     </row>
     <row r="93" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="B93" s="10" t="s">
-        <v>52</v>
+      <c r="A93" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B93" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C93" s="4">
         <v>255</v>
       </c>
-      <c r="D93" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E93" s="10" t="s">
-        <v>17</v>
+      <c r="D93" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E93" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F93" s="5"/>
       <c r="G93" s="5"/>
       <c r="H93" s="5"/>
     </row>
     <row r="94" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="9" t="s">
+      <c r="A94" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B94" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="B94" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="C94" s="4"/>
-      <c r="D94" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E94" s="10" t="s">
+      <c r="D94" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E94" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F94" s="5"/>
@@ -2242,61 +2336,909 @@
       <c r="H94" s="5"/>
     </row>
     <row r="95" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B95" s="10" t="s">
-        <v>82</v>
+      <c r="A95" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B95" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C95" s="4"/>
-      <c r="D95" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="E95" s="10" t="s">
-        <v>26</v>
+      <c r="D95" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E95" s="7" t="s">
+        <v>25</v>
       </c>
       <c r="F95" s="5"/>
       <c r="G95" s="5"/>
       <c r="H95" s="5"/>
     </row>
     <row r="96" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A96" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B96" s="10" t="s">
-        <v>82</v>
+      <c r="A96" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B96" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C96" s="4"/>
-      <c r="D96" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E96" s="10" t="s">
-        <v>17</v>
+      <c r="D96" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F96" s="5"/>
       <c r="G96" s="5"/>
       <c r="H96" s="5"/>
     </row>
     <row r="97" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B97" s="10" t="s">
-        <v>82</v>
+      <c r="A97" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>80</v>
       </c>
       <c r="C97" s="4"/>
-      <c r="D97" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>17</v>
+      <c r="D97" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="F97" s="5"/>
       <c r="G97" s="5"/>
       <c r="H97" s="5"/>
     </row>
+    <row r="100" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B100" s="10"/>
+      <c r="C100" s="10"/>
+      <c r="D100" s="10"/>
+      <c r="E100" s="10"/>
+      <c r="F100" s="10"/>
+      <c r="G100" s="10"/>
+      <c r="H100" s="11"/>
+    </row>
+    <row r="101" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B101" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D101" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G101" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H101" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" s="8"/>
+      <c r="D102" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E102" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F102" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G102" s="4"/>
+      <c r="H102" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C103" s="8">
+        <v>16</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E103" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F103" s="4"/>
+      <c r="G103" s="4"/>
+      <c r="H103" s="4"/>
+    </row>
+    <row r="105" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B105" s="10"/>
+      <c r="C105" s="10"/>
+      <c r="D105" s="10"/>
+      <c r="E105" s="10"/>
+      <c r="F105" s="10"/>
+      <c r="G105" s="10"/>
+      <c r="H105" s="11"/>
+    </row>
+    <row r="106" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A106" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B106" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D106" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E106" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G106" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H106" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A107" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B107" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C107" s="8"/>
+      <c r="D107" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E107" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G107" s="4"/>
+      <c r="H107" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A108" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C108" s="8">
+        <v>16</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F108" s="4"/>
+      <c r="G108" s="4"/>
+      <c r="H108" s="4"/>
+    </row>
+    <row r="111" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A111" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="B111" s="10"/>
+      <c r="C111" s="10"/>
+      <c r="D111" s="10"/>
+      <c r="E111" s="10"/>
+      <c r="F111" s="10"/>
+      <c r="G111" s="10"/>
+      <c r="H111" s="11"/>
+    </row>
+    <row r="112" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D112" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E112" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F112" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G112" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H112" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C113" s="8"/>
+      <c r="D113" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E113" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G113" s="4"/>
+      <c r="H113" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B114" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C114" s="8"/>
+      <c r="D114" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E114" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F114" s="4"/>
+      <c r="G114" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H114" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F115" s="5"/>
+      <c r="G115" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H115" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A116" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C116" s="4">
+        <v>50</v>
+      </c>
+      <c r="D116" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E116" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F116" s="5"/>
+      <c r="G116" s="5"/>
+      <c r="H116" s="8"/>
+    </row>
+    <row r="117" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C117" s="4">
+        <v>255</v>
+      </c>
+      <c r="D117" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E117" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F117" s="5"/>
+      <c r="G117" s="5"/>
+      <c r="H117" s="8"/>
+    </row>
+    <row r="118" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A118" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="B118" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E118" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F118" s="5"/>
+      <c r="G118" s="5"/>
+      <c r="H118" s="8"/>
+    </row>
+    <row r="119" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C119" s="4"/>
+      <c r="D119" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E119" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F119" s="5"/>
+      <c r="G119" s="5"/>
+      <c r="H119" s="8"/>
+    </row>
+    <row r="120" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C120" s="4">
+        <v>255</v>
+      </c>
+      <c r="D120" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E120" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F120" s="5"/>
+      <c r="G120" s="5"/>
+      <c r="H120" s="5"/>
+    </row>
+    <row r="123" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A123" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B123" s="10"/>
+      <c r="C123" s="10"/>
+      <c r="D123" s="10"/>
+      <c r="E123" s="10"/>
+      <c r="F123" s="10"/>
+      <c r="G123" s="10"/>
+      <c r="H123" s="11"/>
+    </row>
+    <row r="124" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D124" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G124" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H124" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C125" s="8"/>
+      <c r="D125" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E125" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F125" s="4"/>
+      <c r="G125" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C126" s="8"/>
+      <c r="D126" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E126" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F126" s="4"/>
+      <c r="G126" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C127" s="4"/>
+      <c r="D127" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="F127" s="5"/>
+      <c r="G127" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="H127" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C128" s="4"/>
+      <c r="D128" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E128" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F128" s="5"/>
+      <c r="G128" s="5"/>
+      <c r="H128" s="8"/>
+    </row>
+    <row r="131" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B131" s="10"/>
+      <c r="C131" s="10"/>
+      <c r="D131" s="10"/>
+      <c r="E131" s="10"/>
+      <c r="F131" s="10"/>
+      <c r="G131" s="10"/>
+      <c r="H131" s="11"/>
+    </row>
+    <row r="132" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B132" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C132" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E132" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F132" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G132" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H132" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C133" s="8"/>
+      <c r="D133" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E133" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F133" s="4"/>
+      <c r="G133" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H133" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B134" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C134" s="8"/>
+      <c r="D134" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E134" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F134" s="4"/>
+      <c r="G134" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H134" s="7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C135" s="4"/>
+      <c r="D135" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F135" s="5"/>
+      <c r="G135" s="5"/>
+      <c r="H135" s="5"/>
+    </row>
+    <row r="136" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B136" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C136" s="4"/>
+      <c r="D136" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E136" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F136" s="5"/>
+      <c r="G136" s="5"/>
+      <c r="H136" s="8"/>
+    </row>
+    <row r="137" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A137" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C137" s="4"/>
+      <c r="D137" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E137" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F137" s="5"/>
+      <c r="G137" s="5"/>
+      <c r="H137" s="8"/>
+    </row>
+    <row r="138" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A138" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B138" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C138" s="4">
+        <v>255</v>
+      </c>
+      <c r="D138" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E138" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F138" s="5"/>
+      <c r="G138" s="5"/>
+      <c r="H138" s="8"/>
+    </row>
+    <row r="141" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B141" s="10"/>
+      <c r="C141" s="10"/>
+      <c r="D141" s="10"/>
+      <c r="E141" s="10"/>
+      <c r="F141" s="10"/>
+      <c r="G141" s="10"/>
+      <c r="H141" s="11"/>
+    </row>
+    <row r="142" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A142" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B142" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C142" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F142" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H142" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A143" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C143" s="8"/>
+      <c r="D143" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E143" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F143" s="4"/>
+      <c r="G143" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="H143" s="8" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A144" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B144" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C144" s="8">
+        <v>30</v>
+      </c>
+      <c r="D144" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E144" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F144" s="4"/>
+      <c r="G144" s="4"/>
+      <c r="H144" s="7"/>
+    </row>
+    <row r="145" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A145" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B145" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C145" s="4">
+        <v>255</v>
+      </c>
+      <c r="D145" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E145" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F145" s="5"/>
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+    </row>
+    <row r="148" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A148" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B148" s="10"/>
+      <c r="C148" s="10"/>
+      <c r="D148" s="10"/>
+      <c r="E148" s="10"/>
+      <c r="F148" s="10"/>
+      <c r="G148" s="10"/>
+      <c r="H148" s="11"/>
+    </row>
+    <row r="149" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A149" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B149" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C149" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D149" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E149" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F149" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G149" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H149" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A150" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C150" s="8"/>
+      <c r="D150" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E150" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F150" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="G150" s="4"/>
+      <c r="H150" s="8" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A151" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C151" s="8"/>
+      <c r="D151" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F151" s="4"/>
+      <c r="G151" s="4"/>
+      <c r="H151" s="7"/>
+    </row>
+    <row r="152" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A152" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B152" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C152" s="8"/>
+      <c r="D152" s="7"/>
+      <c r="E152" s="7"/>
+      <c r="F152" s="4"/>
+      <c r="G152" s="4"/>
+      <c r="H152" s="7"/>
+    </row>
+    <row r="153" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A153" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B153" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C153" s="4"/>
+      <c r="D153" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F153" s="5"/>
+      <c r="G153" s="5"/>
+      <c r="H153" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="15">
     <mergeCell ref="A61:H61"/>
     <mergeCell ref="A69:H69"/>
     <mergeCell ref="A77:H77"/>
@@ -2305,6 +3247,13 @@
     <mergeCell ref="A25:H25"/>
     <mergeCell ref="A48:H48"/>
     <mergeCell ref="A55:H55"/>
+    <mergeCell ref="A141:H141"/>
+    <mergeCell ref="A148:H148"/>
+    <mergeCell ref="A100:H100"/>
+    <mergeCell ref="A105:H105"/>
+    <mergeCell ref="A111:H111"/>
+    <mergeCell ref="A123:H123"/>
+    <mergeCell ref="A131:H131"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>